<commit_message>
use US data for indst/FLRbI
</commit_message>
<xml_diff>
--- a/InputData/indst/FLRbI/Foreign Leakage Rate by Industry.xlsx
+++ b/InputData/indst/FLRbI/Foreign Leakage Rate by Industry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\indst\FLRbI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\Documents\Energy Policy Simulator\Models\eps-eu\InputData\indst\FLRbI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789840D7-2404-480A-8F40-C7CD3E312472}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6813CBAE-247D-4BA0-95F7-2F6B39AFB9B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3915" yWindow="1065" windowWidth="23805" windowHeight="15630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14130" yWindow="-17025" windowWidth="18390" windowHeight="16365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="114">
   <si>
     <t>Source:</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>We take an average of other manufacturing categories here to avoid an unrealistic outlier (170.5% leakage rate)</t>
+  </si>
+  <si>
+    <t>The EU EPS uses values from the US EPS.</t>
   </si>
 </sst>
 </file>
@@ -491,14 +494,14 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -839,22 +842,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.3984375" customWidth="1"/>
+    <col min="3" max="3" width="26.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,261 +867,269 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="2">
         <v>2010</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B37" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B38" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B43" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B44" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B45" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B46" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B47" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A49" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B50" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B51" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B52" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B53" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B55" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B56" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B57" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B58" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B59" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B60" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B61" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B62" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B63" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1135,24 +1148,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="42.28515625" customWidth="1"/>
-    <col min="2" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="42.265625" customWidth="1"/>
+    <col min="2" max="3" width="15.1328125" customWidth="1"/>
+    <col min="4" max="4" width="17.86328125" customWidth="1"/>
+    <col min="5" max="5" width="18.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="14"/>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="15" t="s">
         <v>33</v>
       </c>
@@ -1172,7 +1185,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1192,11 +1205,11 @@
         <v>22</v>
       </c>
       <c r="G3" s="13">
-        <f t="shared" ref="G3:G17" si="0">-F3/B3</f>
+        <f t="shared" ref="G3:G16" si="0">-F3/B3</f>
         <v>2.9502480890438512E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1220,7 +1233,7 @@
         <v>4.1733547351524881E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1244,7 +1257,7 @@
         <v>9.4637223974763401E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1268,7 +1281,7 @@
         <v>-1.799775028121485E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1292,7 +1305,7 @@
         <v>9.958401613513173E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1316,7 +1329,7 @@
         <v>8.2506640646175536E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1340,7 +1353,7 @@
         <v>0.26460159229276781</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1364,7 +1377,7 @@
         <v>9.50544015825915E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1388,7 +1401,7 @@
         <v>0.14969670710571925</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1412,7 +1425,7 @@
         <v>0.13454146073585943</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1436,7 +1449,7 @@
         <v>1.1881188118811881E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1460,7 +1473,7 @@
         <v>4.8814504881450485E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1484,7 +1497,7 @@
         <v>0.13286713286713286</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1508,7 +1521,7 @@
         <v>2.0053475935828879E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1527,7 +1540,7 @@
       <c r="F17" s="14">
         <v>312</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="17">
         <f>AVERAGE(G3:G16)</f>
         <v>7.2094113727029757E-2</v>
       </c>
@@ -1535,7 +1548,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1559,7 +1572,7 @@
         <v>5.884174667079591E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1583,7 +1596,7 @@
         <v>-0.20980392156862746</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1607,7 +1620,7 @@
         <v>-0.62931034482758619</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1631,7 +1644,7 @@
         <v>-1.9602803738317758</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1655,7 +1668,7 @@
         <v>0.81818181818181823</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1679,7 +1692,7 @@
         <v>3.0687218761237403E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1703,7 +1716,7 @@
         <v>1.5285845307245491E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1727,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -1751,7 +1764,7 @@
         <v>-7.3488884806173071E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1775,7 +1788,7 @@
         <v>6.0357972966971145E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1799,7 +1812,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1823,7 +1836,7 @@
         <v>-3.6275695284159614E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1847,7 +1860,7 @@
         <v>1.2755958375293723E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
@@ -1869,13 +1882,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="46.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="46.1328125" customWidth="1"/>
+    <col min="2" max="2" width="17.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>110</v>
       </c>
@@ -1883,7 +1896,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -1892,7 +1905,7 @@
         <v>5.884174667079591E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -1901,7 +1914,7 @@
         <v>-0.20980392156862746</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1910,7 +1923,7 @@
         <v>-0.85572337042925273</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -1919,7 +1932,7 @@
         <v>0.81818181818181823</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -1928,7 +1941,7 @@
         <v>2.9502480890438512E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -1937,7 +1950,7 @@
         <v>9.4637223974763401E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1946,7 +1959,7 @@
         <v>-1.799775028121485E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>92</v>
       </c>
@@ -1955,7 +1968,7 @@
         <v>9.958401613513173E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>93</v>
       </c>
@@ -1964,7 +1977,7 @@
         <v>8.2506640646175536E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -1973,7 +1986,7 @@
         <v>0.26460159229276781</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>95</v>
       </c>
@@ -1982,7 +1995,7 @@
         <v>0.26460159229276781</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -1991,7 +2004,7 @@
         <v>9.50544015825915E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -2000,7 +2013,7 @@
         <v>9.50544015825915E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -2009,7 +2022,7 @@
         <v>0.14969670710571925</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>99</v>
       </c>
@@ -2018,7 +2031,7 @@
         <v>0.13454146073585943</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>100</v>
       </c>
@@ -2027,7 +2040,7 @@
         <v>1.1881188118811881E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>101</v>
       </c>
@@ -2036,7 +2049,7 @@
         <v>0.13286713286713286</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>102</v>
       </c>
@@ -2045,7 +2058,7 @@
         <v>0.13286713286713286</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -2054,7 +2067,7 @@
         <v>2.0053475935828879E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>104</v>
       </c>
@@ -2063,7 +2076,7 @@
         <v>4.8814504881450485E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>105</v>
       </c>
@@ -2072,7 +2085,7 @@
         <v>4.8814504881450485E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -2081,7 +2094,7 @@
         <v>7.2094113727029757E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>107</v>
       </c>
@@ -2090,7 +2103,7 @@
         <v>1.5285845307245491E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>108</v>
       </c>
@@ -2098,11 +2111,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>109</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="18">
         <f>SourceData!G25</f>
         <v>0</v>
       </c>

</xml_diff>